<commit_message>
Fixed issue of comments not being taken from the sheet that they belong to
</commit_message>
<xml_diff>
--- a/test/test_resources/comments.xlsx
+++ b/test/test_resources/comments.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\excel\test\test_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09914C2B-092E-4FE6-8908-6CC769C79A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE3FAB5-1A9D-4C80-811F-D6F06EE15344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11895" yWindow="2295" windowWidth="21600" windowHeight="11295" xr2:uid="{53A650A5-FA65-429E-86B0-D1D0EE927C85}"/>
+    <workbookView xWindow="7170" yWindow="1140" windowWidth="21600" windowHeight="11295" xr2:uid="{53A650A5-FA65-429E-86B0-D1D0EE927C85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Different Name" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,11 +49,11 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>This is a random sample comment</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{4368BF88-45B7-4F38-8ABF-D8280F5984C9}">
+          <t>A2Sheet1: This is a random sample comment</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{46BC50FD-A920-4B88-B074-7703B70983E7}">
       <text>
         <r>
           <rPr>
@@ -62,7 +63,21 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Another comment</t>
+          <t>B2Sheet1: Empty Value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{4368BF88-45B7-4F38-8ABF-D8280F5984C9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>A3Sheet1: Another comment</t>
         </r>
       </text>
     </comment>
@@ -75,7 +90,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>Comment with different font and size</t>
+          <t>A5Sheet1: Comment with different font and size</t>
         </r>
       </text>
     </comment>
@@ -83,8 +98,86 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Aesreal</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{5BE0F31D-5D49-4B31-8C0A-88324A236066}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>A2DN: Empty Value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{9B25A024-92C2-44C3-B411-1C2B808D19C7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>B2DN: Random Comment</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{41B44CDE-4745-4D12-A1B6-B6EEF916E5FC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>A3DN: Another comment</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{D7E418A4-8368-4D36-813B-E96C27AD63E2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>C3DN: C3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{5F0A1C94-434B-46D2-A4C7-4ECB4FC8CE66}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>A5DN: Comment with different font and size</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Value 1</t>
   </si>
@@ -99,6 +192,21 @@
   </si>
   <si>
     <t>Value 5</t>
+  </si>
+  <si>
+    <t>1 Value</t>
+  </si>
+  <si>
+    <t>2 Value</t>
+  </si>
+  <si>
+    <t>3 Value</t>
+  </si>
+  <si>
+    <t>4 Value</t>
+  </si>
+  <si>
+    <t>5 Value</t>
   </si>
 </sst>
 </file>
@@ -469,33 +577,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30EAFC4C-671E-4207-B1AB-C3DF59392432}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -505,4 +613,52 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82417EBC-FAFD-47F8-B0F9-D5A265843888}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>